<commit_message>
work on glancing angle macro builder
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">Pinwheel</t>
+  </si>
   <si>
     <t xml:space="preserve">Experimenters:</t>
   </si>
@@ -67,7 +70,7 @@
     <t xml:space="preserve">Ancillary information</t>
   </si>
   <si>
-    <t xml:space="preserve">Slot number</t>
+    <t xml:space="preserve">Spinner number</t>
   </si>
   <si>
     <t xml:space="preserve">Measure this spinner?</t>
@@ -864,9 +867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>302400</xdr:colOff>
+      <xdr:colOff>301680</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -876,7 +879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="6643800" cy="1809360"/>
+          <a:ext cx="6643080" cy="1808640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1058,11 +1061,48 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>110880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>42840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4041360"/>
+          <a:ext cx="2743200" cy="2532960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1073,33 +1113,39 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="R21" activeCellId="0" sqref="R21"/>
+      <selection pane="bottomRight" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
@@ -1129,25 +1175,25 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="E2" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1185,39 +1231,39 @@
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
       <c r="U4" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
@@ -1225,148 +1271,148 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB4" s="15"/>
       <c r="AC4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K5" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N5" s="24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S5" s="26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T5" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U5" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V5" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W5" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X5" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y5" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA5" s="20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AC5" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" s="28" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K6" s="36" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M6" s="38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N6" s="39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O6" s="40" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P6" s="41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R6" s="43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -1403,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="50"/>
       <c r="E7" s="4"/>
@@ -1433,7 +1479,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="4"/>
@@ -1463,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="4"/>
@@ -1493,7 +1539,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="4"/>
@@ -1523,7 +1569,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="4"/>
@@ -1553,7 +1599,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="4"/>
@@ -1583,7 +1629,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="4"/>
@@ -1613,7 +1659,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="4"/>

</xml_diff>

<commit_message>
adjust size of photo in pinwheel spreadsheet template
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -867,9 +867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:colOff>301320</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -879,7 +879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="6643080" cy="1808640"/>
+          <a:ext cx="6642720" cy="1808280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1065,14 +1065,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>171000</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1085,7 +1085,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4041360"/>
+          <a:off x="0" y="4093200"/>
           <a:ext cx="2743200" cy="2532960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1102,42 +1102,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:AC38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
more work on glancing angle automation + generalized xlsx() command
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -19,10 +19,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell!</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
-  <si>
-    <t xml:space="preserve">Pinwheel</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">Glancing angle</t>
   </si>
   <si>
     <t xml:space="preserve">Experimenters:</t>
@@ -50,9 +73,6 @@
   </si>
   <si>
     <t xml:space="preserve">Photon delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glancing angle</t>
   </si>
   <si>
     <t xml:space="preserve">Sample metadata</t>
@@ -867,9 +887,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
+      <xdr:colOff>300960</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -879,7 +899,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="6643080" cy="1808640"/>
+          <a:ext cx="6642360" cy="1807920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1070,9 +1090,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>171000</xdr:colOff>
+      <xdr:colOff>170280</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1086,7 +1106,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4041360"/>
-          <a:ext cx="2743200" cy="2532960"/>
+          <a:ext cx="2742480" cy="2532240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1113,7 +1133,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1245,25 +1265,25 @@
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
       <c r="K4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>11</v>
       </c>
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
       <c r="O4" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
       <c r="R4" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
       <c r="U4" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
@@ -1271,148 +1291,148 @@
       <c r="Y4" s="14"/>
       <c r="Z4" s="14"/>
       <c r="AA4" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB4" s="15"/>
       <c r="AC4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="I5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="K5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="L5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="M5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="N5" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="O5" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="P5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="Q5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="R5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="U5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="U5" s="17" t="s">
+      <c r="V5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="W5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="X5" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="X5" s="16" t="s">
+      <c r="Y5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Z5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="AA5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AA5" s="20" t="s">
+      <c r="AB5" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AB5" s="27" t="s">
+      <c r="AC5" s="27" t="s">
         <v>42</v>
-      </c>
-      <c r="AC5" s="27" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" s="28" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="29" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" s="33" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="J6" s="36" t="s">
         <v>48</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>49</v>
       </c>
       <c r="K6" s="36" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="N6" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="O6" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="P6" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="Q6" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="R6" s="43" t="s">
         <v>55</v>
-      </c>
-      <c r="R6" s="43" t="s">
-        <v>56</v>
       </c>
       <c r="S6" s="42"/>
       <c r="T6" s="42"/>
@@ -1832,6 +1852,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more work incorporating glancing angle stage
and having it live gracefully with the sample wheel and future instruments
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -43,12 +43,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t xml:space="preserve">Glancing angle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experimenters:</t>
   </si>
   <si>
     <t xml:space="preserve">Change edge at start?</t>
@@ -310,12 +307,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -559,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -568,11 +571,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,7 +587,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,8 +595,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -600,27 +611,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -676,79 +687,79 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -852,7 +863,7 @@
       <rgbColor rgb="FFCFF660"/>
       <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
@@ -882,14 +893,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>666360</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>300600</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:colOff>1477440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>80280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -899,7 +910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="6642000" cy="1807560"/>
+          <a:ext cx="7818840" cy="1806480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1033,7 +1044,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Specify motor positions and the method for finding them in columns P,Q,R</a:t>
+            <a:t>5. Specify pitch and y motor positions and the method for finding them in columns P,Q,R</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1071,7 +1082,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column AA</a:t>
+            <a:t>7. Do not add columns before column AC</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1090,9 +1101,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>169920</xdr:colOff>
+      <xdr:colOff>168840</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1105,8 +1116,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="4041360"/>
-          <a:ext cx="2742120" cy="2531880"/>
+          <a:off x="0" y="4181760"/>
+          <a:ext cx="2741040" cy="2530800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1161,627 +1172,624 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
       <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="9"/>
+      <c r="L2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="11"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
-      <c r="Z2" s="9"/>
+      <c r="Z2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="9"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="11"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
-      <c r="Z3" s="9"/>
+      <c r="Z3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="14" t="s">
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14" t="s">
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14" t="s">
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14" t="s">
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="15" t="s">
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-    </row>
-    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="F5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="G5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="I5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="K5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="L5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="M5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="N5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="O5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="23" t="s">
+      <c r="P5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="Q5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="R5" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="S5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="18" t="s">
+      <c r="U5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="17" t="s">
+      <c r="V5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="W5" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="X5" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="16" t="s">
+      <c r="Y5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Z5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="AA5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="20" t="s">
+      <c r="AB5" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="27" t="s">
+      <c r="AC5" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="27" t="s">
+    </row>
+    <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" s="28" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="29" t="s">
+      <c r="C6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="31" t="s">
+      <c r="E6" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="32" t="s">
+      <c r="G6" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="34" t="s">
+      <c r="I6" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="J6" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="K6" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" s="37" t="s">
+      <c r="M6" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="N6" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="O6" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="P6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="Q6" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="R6" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="44" t="n">
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="46" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="45" t="n">
+      <c r="V6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="45" t="n">
+      <c r="W6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="45" t="n">
+      <c r="X6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="45" t="n">
+      <c r="Y6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="46" t="n">
+      <c r="Z6" s="48" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="n">
+      <c r="B7" s="50" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="57"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="60"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="60"/>
+      <c r="Y7" s="60"/>
+      <c r="Z7" s="61"/>
+      <c r="AA7" s="62"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="57"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="60"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="61"/>
+      <c r="AA8" s="62"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="50" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="57"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="60"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="60"/>
+      <c r="Y9" s="60"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="62"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="50" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="57"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="60"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="61"/>
+      <c r="AA10" s="62"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="50" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="55"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="57"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="59"/>
-      <c r="AA7" s="60"/>
-    </row>
-    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="48" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="55"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="57"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-      <c r="Z8" s="59"/>
-      <c r="AA8" s="60"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="48" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="55"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="57"/>
-      <c r="V9" s="58"/>
-      <c r="W9" s="58"/>
-      <c r="X9" s="58"/>
-      <c r="Y9" s="58"/>
-      <c r="Z9" s="59"/>
-      <c r="AA9" s="60"/>
-    </row>
-    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="48" t="n">
+      <c r="C11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="55"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="57"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="58"/>
-      <c r="Z10" s="59"/>
-      <c r="AA10" s="60"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="48" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="55"/>
-      <c r="T11" s="56"/>
-      <c r="U11" s="57"/>
-      <c r="V11" s="58"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="58"/>
-      <c r="Y11" s="58"/>
-      <c r="Z11" s="59"/>
-      <c r="AA11" s="60"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="57"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="61"/>
+      <c r="AA11" s="62"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="48" t="n">
+      <c r="B12" s="50" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="55"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="57"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
-      <c r="Y12" s="58"/>
-      <c r="Z12" s="59"/>
-      <c r="AA12" s="60"/>
+      <c r="C12" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="57"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="61"/>
+      <c r="AA12" s="62"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="48" t="n">
+      <c r="B13" s="50" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="55"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="57"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="58"/>
-      <c r="X13" s="58"/>
-      <c r="Y13" s="58"/>
-      <c r="Z13" s="59"/>
-      <c r="AA13" s="60"/>
+      <c r="C13" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="57"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="60"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="61"/>
+      <c r="AA13" s="62"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="48" t="n">
+      <c r="B14" s="50" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="55"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="57"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="58"/>
-      <c r="X14" s="58"/>
-      <c r="Y14" s="58"/>
-      <c r="Z14" s="59"/>
-      <c r="AA14" s="60"/>
+      <c r="C14" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="57"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="57"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="60"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="60"/>
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="61"/>
+      <c r="AA14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="48"/>
+      <c r="B15" s="50"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="48"/>
+      <c r="B16" s="50"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="48"/>
+      <c r="B17" s="50"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="48"/>
+      <c r="B18" s="50"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="48"/>
+      <c r="B19" s="50"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="48"/>
+      <c r="B20" s="50"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="48"/>
+      <c r="B21" s="50"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="48"/>
+      <c r="B22" s="50"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="48"/>
+      <c r="B23" s="50"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="48"/>
+      <c r="B24" s="50"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="48"/>
+      <c r="B25" s="50"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="48"/>
+      <c r="B26" s="50"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="48"/>
+      <c r="B27" s="50"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="48"/>
+      <c r="B28" s="50"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="48"/>
+      <c r="B29" s="50"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="48"/>
+      <c r="B30" s="50"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="48"/>
+      <c r="B31" s="50"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="48"/>
+      <c r="B32" s="50"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="48"/>
+      <c r="B33" s="50"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="48"/>
+      <c r="B34" s="50"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="48"/>
+      <c r="B35" s="50"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="48"/>
+      <c r="B36" s="50"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="48"/>
+      <c r="B37" s="50"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="48"/>
+      <c r="B38" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:Z1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:J4"/>
@@ -1812,7 +1820,7 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2 K2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1828,7 +1836,7 @@
       <formula1>10</formula1>
       <formula2>400</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1840,9 +1848,9 @@
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
       <formula1>0</formula1>
-      <formula2>0</formula2>
+      <formula2>10</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
improvements to spreadsheet automation
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t xml:space="preserve">Glancing angle</t>
   </si>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">XAFS Scan parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">Motor positions for sample flat in beam</t>
+    <t xml:space="preserve">Motor position</t>
   </si>
   <si>
     <t xml:space="preserve">Flags</t>
@@ -174,6 +174,9 @@
     <t xml:space="preserve">Sample y  abs. pos. (mm)</t>
   </si>
   <si>
+    <t xml:space="preserve">Detector X</t>
+  </si>
+  <si>
     <t xml:space="preserve">snapshots</t>
   </si>
   <si>
@@ -248,7 +251,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,8 +309,22 @@
       <name val="Bitstream Vera Sans"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Bitstream Vera Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Bitstream Vera Sans"/>
+      <family val="0"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,7 +340,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF66"/>
-        <bgColor rgb="FFCFF660"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -336,12 +353,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCFF660"/>
-        <bgColor rgb="FFCCFF66"/>
       </patternFill>
     </fill>
   </fills>
@@ -562,7 +573,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -571,7 +582,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -743,8 +754,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -860,7 +875,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCFF660"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99FF"/>
@@ -898,9 +913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1477440</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -910,7 +925,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="7818840" cy="1806480"/>
+          <a:ext cx="7818120" cy="2244960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1044,7 +1059,7 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>5. Specify pitch and y motor positions and the method for finding them in columns P,Q,R</a:t>
+            <a:t>5. Specify pitch and y motor positions and the method for finding them in columns R, S, T</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1063,7 +1078,25 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>6. Do not add rows above row 7</a:t>
+            <a:t>6. If column R is “Manual”, columns S and T </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>must</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> be filled in</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1082,7 +1115,63 @@
               </a:solidFill>
               <a:latin typeface="Bitstream Vera Sans"/>
             </a:rPr>
-            <a:t>7. Do not add columns before column AC</a:t>
+            <a:t>7. Specify detector position in column U, blank means to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>not move</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> detector</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>8. Do not add rows above row 7</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>9. Do not add columns before column AE</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:latin typeface="Times New Roman"/>
@@ -1101,9 +1190,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>168840</xdr:colOff>
+      <xdr:colOff>168120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1117,7 +1206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2741040" cy="2530800"/>
+          <a:ext cx="2740320" cy="2530080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1137,14 +1226,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AC38"/>
+  <dimension ref="B1:AD38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1164,11 +1253,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1199,6 +1289,7 @@
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5"/>
@@ -1228,12 +1319,13 @@
       <c r="R2" s="10"/>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="0"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="11"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
-      <c r="Z2" s="11"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5"/>
@@ -1249,12 +1341,13 @@
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="0"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="11"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
-      <c r="Z3" s="11"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
@@ -1290,19 +1383,20 @@
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="U4" s="16"/>
+      <c r="V4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="V4" s="16"/>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
-      <c r="AA4" s="17" t="s">
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="AB4" s="17"/>
       <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
@@ -1362,10 +1456,10 @@
       <c r="T5" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="V5" s="18" t="s">
+      <c r="V5" s="19" t="s">
         <v>34</v>
       </c>
       <c r="W5" s="18" t="s">
@@ -1377,90 +1471,90 @@
       <c r="Y5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="24" t="s">
+      <c r="Z5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="AA5" s="22" t="s">
+      <c r="AA5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AB5" s="22" t="s">
         <v>40</v>
       </c>
       <c r="AC5" s="29" t="s">
         <v>41</v>
       </c>
+      <c r="AD5" s="29" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E6" s="31" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K6" s="38" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M6" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N6" s="41" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q6" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R6" s="45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="46" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T6" s="46"/>
+      <c r="U6" s="44"/>
       <c r="V6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="47" t="n">
+      <c r="W6" s="48" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="47" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="47" t="n">
+      <c r="X6" s="48" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="48" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1468,326 +1562,338 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="49"/>
-      <c r="AB6" s="44"/>
+      <c r="AA6" s="49" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="50"/>
       <c r="AC6" s="44"/>
+      <c r="AD6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="50" t="n">
+      <c r="B7" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="53"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="57"/>
-      <c r="O7" s="56"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="57"/>
       <c r="P7" s="30"/>
-      <c r="Q7" s="57"/>
-      <c r="T7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="59"/>
       <c r="V7" s="60"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="60"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
       <c r="Z7" s="61"/>
       <c r="AA7" s="62"/>
+      <c r="AB7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="50" t="n">
+      <c r="B8" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="56"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="57"/>
       <c r="P8" s="30"/>
-      <c r="Q8" s="57"/>
-      <c r="T8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="T8" s="10"/>
       <c r="U8" s="59"/>
       <c r="V8" s="60"/>
-      <c r="W8" s="60"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="60"/>
+      <c r="W8" s="61"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="61"/>
       <c r="Z8" s="61"/>
       <c r="AA8" s="62"/>
+      <c r="AB8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="50" t="n">
+      <c r="B9" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="56"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="57"/>
       <c r="P9" s="30"/>
-      <c r="Q9" s="57"/>
-      <c r="T9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="T9" s="10"/>
       <c r="U9" s="59"/>
       <c r="V9" s="60"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="60"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
       <c r="Z9" s="61"/>
       <c r="AA9" s="62"/>
+      <c r="AB9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="50" t="n">
+      <c r="B10" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="56"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="57"/>
       <c r="P10" s="30"/>
-      <c r="Q10" s="57"/>
-      <c r="T10" s="58"/>
+      <c r="Q10" s="58"/>
+      <c r="T10" s="10"/>
       <c r="U10" s="59"/>
       <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="61"/>
       <c r="Z10" s="61"/>
       <c r="AA10" s="62"/>
+      <c r="AB10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="50" t="n">
+      <c r="B11" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="56"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="57"/>
       <c r="P11" s="30"/>
-      <c r="Q11" s="57"/>
-      <c r="T11" s="58"/>
+      <c r="Q11" s="58"/>
+      <c r="T11" s="10"/>
       <c r="U11" s="59"/>
       <c r="V11" s="60"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="60"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
       <c r="Z11" s="61"/>
       <c r="AA11" s="62"/>
+      <c r="AB11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="50" t="n">
+      <c r="B12" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="56"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="57"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="57"/>
       <c r="P12" s="30"/>
-      <c r="Q12" s="57"/>
-      <c r="T12" s="58"/>
+      <c r="Q12" s="58"/>
+      <c r="T12" s="10"/>
       <c r="U12" s="59"/>
       <c r="V12" s="60"/>
-      <c r="W12" s="60"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="60"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="61"/>
       <c r="Z12" s="61"/>
       <c r="AA12" s="62"/>
+      <c r="AB12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="50" t="n">
+      <c r="B13" s="51" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="57"/>
-      <c r="O13" s="56"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="57"/>
       <c r="P13" s="30"/>
-      <c r="Q13" s="57"/>
-      <c r="T13" s="58"/>
+      <c r="Q13" s="58"/>
+      <c r="T13" s="10"/>
       <c r="U13" s="59"/>
       <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="60"/>
+      <c r="W13" s="61"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="61"/>
       <c r="Z13" s="61"/>
       <c r="AA13" s="62"/>
+      <c r="AB13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="50" t="n">
+      <c r="B14" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="52" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="56"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="57"/>
       <c r="P14" s="30"/>
-      <c r="Q14" s="57"/>
-      <c r="T14" s="58"/>
+      <c r="Q14" s="58"/>
+      <c r="T14" s="10"/>
       <c r="U14" s="59"/>
       <c r="V14" s="60"/>
-      <c r="W14" s="60"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="60"/>
+      <c r="W14" s="61"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="61"/>
       <c r="Z14" s="61"/>
       <c r="AA14" s="62"/>
+      <c r="AB14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="50"/>
+      <c r="B15" s="51"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="50"/>
+      <c r="B16" s="51"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="50"/>
+      <c r="B17" s="51"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="50"/>
+      <c r="B18" s="51"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="50"/>
+      <c r="B19" s="51"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="50"/>
+      <c r="B20" s="51"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="50"/>
+      <c r="B21" s="51"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="50"/>
+      <c r="B22" s="51"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="50"/>
+      <c r="B23" s="51"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="50"/>
+      <c r="B24" s="51"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="50"/>
+      <c r="B25" s="51"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="50"/>
+      <c r="B26" s="51"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="50"/>
+      <c r="B27" s="51"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="50"/>
+      <c r="B28" s="51"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="50"/>
+      <c r="B29" s="51"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="50"/>
+      <c r="B30" s="51"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="50"/>
+      <c r="B31" s="51"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="50"/>
+      <c r="B32" s="51"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="50"/>
+      <c r="B33" s="51"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="50"/>
+      <c r="B34" s="51"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="50"/>
+      <c r="B35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="50"/>
+      <c r="B36" s="51"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="50"/>
+      <c r="B37" s="51"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="50"/>
+      <c r="B38" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:Z1"/>
+    <mergeCell ref="E1:AA1"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
@@ -1795,12 +1901,12 @@
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="U4:Z4"/>
-    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="13">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:Z14" type="list">
+  <dataValidations count="14">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1828,7 +1934,7 @@
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AA6:AC6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
@@ -1852,6 +1958,10 @@
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:U14" type="decimal">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fixed a small spreadsheet bug
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -43,9 +43,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t xml:space="preserve">Glancing angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experimenters:</t>
   </si>
   <si>
     <t xml:space="preserve">Change edge at start?</t>
@@ -913,9 +916,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1476720</xdr:colOff>
+      <xdr:colOff>1476360</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -925,7 +928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3238560" y="4295160"/>
-          <a:ext cx="7818120" cy="2244960"/>
+          <a:ext cx="7817760" cy="2244600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1190,9 +1193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>168120</xdr:colOff>
+      <xdr:colOff>167760</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>39960</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1206,7 +1209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2740320" cy="2530080"/>
+          <a:ext cx="2739960" cy="2529720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1222,7 +1225,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1233,32 +1236,29 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q6" activeCellId="0" sqref="Q6"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1266,7 +1266,9 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -1295,24 +1297,24 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O2" s="10"/>
       <c r="Q2" s="10"/>
@@ -1352,16 +1354,16 @@
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -1369,23 +1371,23 @@
         <v>0</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
       <c r="O4" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P4" s="16"/>
       <c r="Q4" s="16"/>
       <c r="R4" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S4" s="16"/>
       <c r="T4" s="16"/>
       <c r="U4" s="16"/>
       <c r="V4" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="16"/>
@@ -1393,151 +1395,151 @@
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
       <c r="AB4" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AC4" s="17"/>
       <c r="AD4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R5" s="27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T5" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U5" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="X5" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Y5" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Z5" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AA5" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB5" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AC5" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AD5" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E6" s="31" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K6" s="38" t="n">
         <v>2</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M6" s="40" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N6" s="41" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="44" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R6" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S6" s="44"/>
       <c r="T6" s="46"/>
@@ -1575,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="53"/>
       <c r="E7" s="5"/>
@@ -1606,7 +1608,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="53"/>
       <c r="E8" s="5"/>
@@ -1637,7 +1639,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" s="30"/>
       <c r="E9" s="5"/>
@@ -1668,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="5"/>
@@ -1699,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="5"/>
@@ -1730,7 +1732,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="30"/>
       <c r="E12" s="5"/>
@@ -1761,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="30"/>
       <c r="E13" s="5"/>
@@ -1792,7 +1794,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="5"/>

</xml_diff>

<commit_message>
fixed validities in spreadsheets
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -250,9 +250,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -576,7 +577,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -745,7 +746,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -810,6 +811,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -916,9 +921,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1476360</xdr:colOff>
+      <xdr:colOff>1476000</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -927,8 +932,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3238560" y="4295160"/>
-          <a:ext cx="7817760" cy="2244600"/>
+          <a:off x="3239280" y="4295160"/>
+          <a:ext cx="7818840" cy="2244240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1193,9 +1198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>167760</xdr:colOff>
+      <xdr:colOff>167400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1209,7 +1214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4181760"/>
-          <a:ext cx="2739960" cy="2529720"/>
+          <a:ext cx="2740320" cy="2529360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,10 +1241,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -1590,18 +1595,18 @@
       <c r="L7" s="57"/>
       <c r="M7" s="53"/>
       <c r="N7" s="58"/>
-      <c r="O7" s="57"/>
+      <c r="O7" s="59"/>
       <c r="P7" s="30"/>
       <c r="Q7" s="58"/>
       <c r="T7" s="10"/>
-      <c r="U7" s="59"/>
-      <c r="V7" s="60"/>
-      <c r="W7" s="61"/>
-      <c r="X7" s="61"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="63"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="61"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="51" t="n">
@@ -1621,18 +1626,18 @@
       <c r="L8" s="57"/>
       <c r="M8" s="53"/>
       <c r="N8" s="58"/>
-      <c r="O8" s="57"/>
+      <c r="O8" s="59"/>
       <c r="P8" s="30"/>
       <c r="Q8" s="58"/>
       <c r="T8" s="10"/>
-      <c r="U8" s="59"/>
-      <c r="V8" s="60"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="61"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="62"/>
-      <c r="AB8" s="63"/>
+      <c r="U8" s="60"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="63"/>
+      <c r="AB8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="51" t="n">
@@ -1652,18 +1657,18 @@
       <c r="L9" s="57"/>
       <c r="M9" s="53"/>
       <c r="N9" s="58"/>
-      <c r="O9" s="57"/>
+      <c r="O9" s="59"/>
       <c r="P9" s="30"/>
       <c r="Q9" s="58"/>
       <c r="T9" s="10"/>
-      <c r="U9" s="59"/>
-      <c r="V9" s="60"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="63"/>
+      <c r="U9" s="60"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="51" t="n">
@@ -1683,18 +1688,18 @@
       <c r="L10" s="57"/>
       <c r="M10" s="53"/>
       <c r="N10" s="58"/>
-      <c r="O10" s="57"/>
+      <c r="O10" s="59"/>
       <c r="P10" s="30"/>
       <c r="Q10" s="58"/>
       <c r="T10" s="10"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="61"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="63"/>
+      <c r="U10" s="60"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="63"/>
+      <c r="AB10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="51" t="n">
@@ -1714,18 +1719,18 @@
       <c r="L11" s="57"/>
       <c r="M11" s="53"/>
       <c r="N11" s="58"/>
-      <c r="O11" s="57"/>
+      <c r="O11" s="59"/>
       <c r="P11" s="30"/>
       <c r="Q11" s="58"/>
       <c r="T11" s="10"/>
-      <c r="U11" s="59"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="63"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="63"/>
+      <c r="AB11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="51" t="n">
@@ -1745,18 +1750,18 @@
       <c r="L12" s="57"/>
       <c r="M12" s="53"/>
       <c r="N12" s="58"/>
-      <c r="O12" s="57"/>
+      <c r="O12" s="59"/>
       <c r="P12" s="30"/>
       <c r="Q12" s="58"/>
       <c r="T12" s="10"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="60"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="62"/>
-      <c r="AB12" s="63"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="61"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="63"/>
+      <c r="AB12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="51" t="n">
@@ -1776,18 +1781,18 @@
       <c r="L13" s="57"/>
       <c r="M13" s="53"/>
       <c r="N13" s="58"/>
-      <c r="O13" s="57"/>
+      <c r="O13" s="59"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="58"/>
       <c r="T13" s="10"/>
-      <c r="U13" s="59"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="61"/>
-      <c r="X13" s="61"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="62"/>
-      <c r="AB13" s="63"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="61"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="63"/>
+      <c r="AB13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="51" t="n">
@@ -1807,18 +1812,18 @@
       <c r="L14" s="57"/>
       <c r="M14" s="53"/>
       <c r="N14" s="58"/>
-      <c r="O14" s="57"/>
+      <c r="O14" s="59"/>
       <c r="P14" s="30"/>
       <c r="Q14" s="58"/>
       <c r="T14" s="10"/>
-      <c r="U14" s="59"/>
-      <c r="V14" s="60"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="62"/>
-      <c r="AB14" s="63"/>
+      <c r="U14" s="60"/>
+      <c r="V14" s="61"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="63"/>
+      <c r="AB14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="51"/>
@@ -1907,7 +1912,7 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="14">
+  <dataValidations count="12">
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
@@ -1932,17 +1937,9 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:T14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
-      <formula1>-0.1</formula1>
-      <formula2>8</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="decimal">
-      <formula1>10</formula1>
-      <formula2>400</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
@@ -1960,9 +1957,9 @@
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:U14" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U14" type="none">
       <formula1>10</formula1>
-      <formula2>210</formula2>
+      <formula2>400</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
hide some columns in spreadsheets
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -1237,11 +1237,11 @@
   <dimension ref="B1:AD38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="AE7" activeCellId="0" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1261,9 +1261,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1546,7 +1546,7 @@
       <c r="R6" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="44"/>
+      <c r="S6" s="43"/>
       <c r="T6" s="46"/>
       <c r="U6" s="44"/>
       <c r="V6" s="47" t="n">

</xml_diff>

<commit_message>
xlsx improvment, choose from sheets, versioning
</commit_message>
<xml_diff>
--- a/startup/pinwheel_template.xlsx
+++ b/startup/pinwheel_template.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Version history" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -38,17 +39,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t xml:space="preserve">Glancing angle</t>
   </si>
   <si>
     <t xml:space="preserve">Experimenters:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 5</t>
   </si>
   <si>
     <t xml:space="preserve">Change edge at start?</t>
@@ -245,15 +262,35 @@
   <si>
     <t xml:space="preserve">Automatic</t>
   </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added detector X and ancillary information columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell identifying target instrument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell identifying spreadsheet version number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -328,7 +365,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,14 +386,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE0C2CD"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFE0C2CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFE0C2CD"/>
       </patternFill>
     </fill>
   </fills>
@@ -577,7 +620,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -598,11 +641,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,7 +653,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -626,27 +669,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -746,7 +793,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -814,10 +861,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -836,6 +879,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -872,7 +919,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFE0C2CD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1219,7 +1266,7 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -1237,11 +1284,11 @@
   <dimension ref="B1:AD38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="6" topLeftCell="Q7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="AE7" activeCellId="0" sqref="AE7"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1261,9 +1308,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1299,27 +1346,29 @@
       <c r="AA1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="E2" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O2" s="10"/>
       <c r="Q2" s="10"/>
@@ -1335,8 +1384,8 @@
       <c r="AA2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
       <c r="H3" s="1"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -1358,246 +1407,246 @@
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
-      <c r="C4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14" t="s">
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16" t="s">
+      <c r="L4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16" t="s">
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16" t="s">
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="17" t="s">
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="17"/>
-      <c r="AD4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="G5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="I5" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="J5" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="K5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="L5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="M5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="N5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="O5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="P5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="27" t="s">
+      <c r="Q5" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="28" t="s">
+      <c r="R5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="S5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="20" t="s">
+      <c r="T5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="U5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="V5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="W5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="X5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="18" t="s">
+      <c r="Y5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="24" t="s">
+      <c r="Z5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="22" t="s">
+      <c r="AA5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="29" t="s">
+      <c r="AB5" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AD5" s="29" t="s">
+      <c r="AC5" s="30" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="31" t="s">
+      <c r="AD5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="33" t="s">
+    </row>
+    <row r="6" s="31" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="31" t="n">
+      <c r="C6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="36" t="s">
+      <c r="F6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="37" t="s">
+      <c r="G6" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="I6" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="38" t="n">
+      <c r="J6" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="L6" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="40" t="s">
+      <c r="L6" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="41" t="s">
+      <c r="M6" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="42" t="s">
+      <c r="N6" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="43" t="s">
+      <c r="O6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="44" t="s">
+      <c r="P6" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="Q6" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="43"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="47" t="n">
+      <c r="R6" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" s="45"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="48" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="48" t="n">
+      <c r="W6" s="49" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="48" t="n">
+      <c r="X6" s="49" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="Y6" s="48" t="n">
+      <c r="Y6" s="49" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="48" t="n">
+      <c r="Z6" s="49" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="49" t="n">
+      <c r="AA6" s="50" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="50"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
+      <c r="AB6" s="51"/>
+      <c r="AC6" s="45"/>
+      <c r="AD6" s="45"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="51" t="n">
+      <c r="B7" s="52" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="58"/>
+      <c r="C7" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="59"/>
       <c r="T7" s="10"/>
       <c r="U7" s="60"/>
       <c r="V7" s="61"/>
@@ -1609,26 +1658,26 @@
       <c r="AB7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="51" t="n">
+      <c r="B8" s="52" t="n">
         <v>2</v>
       </c>
-      <c r="C8" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="58"/>
+      <c r="C8" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="59"/>
       <c r="T8" s="10"/>
       <c r="U8" s="60"/>
       <c r="V8" s="61"/>
@@ -1640,26 +1689,26 @@
       <c r="AB8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="51" t="n">
+      <c r="B9" s="52" t="n">
         <v>3</v>
       </c>
-      <c r="C9" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="58"/>
+      <c r="C9" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="59"/>
       <c r="T9" s="10"/>
       <c r="U9" s="60"/>
       <c r="V9" s="61"/>
@@ -1671,26 +1720,26 @@
       <c r="AB9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="51" t="n">
+      <c r="B10" s="52" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="58"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="58"/>
+      <c r="C10" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="59"/>
       <c r="T10" s="10"/>
       <c r="U10" s="60"/>
       <c r="V10" s="61"/>
@@ -1702,26 +1751,26 @@
       <c r="AB10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="51" t="n">
+      <c r="B11" s="52" t="n">
         <v>5</v>
       </c>
-      <c r="C11" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="58"/>
+      <c r="C11" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="59"/>
       <c r="T11" s="10"/>
       <c r="U11" s="60"/>
       <c r="V11" s="61"/>
@@ -1733,26 +1782,26 @@
       <c r="AB11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="51" t="n">
+      <c r="B12" s="52" t="n">
         <v>6</v>
       </c>
-      <c r="C12" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="58"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="58"/>
+      <c r="C12" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="59"/>
       <c r="T12" s="10"/>
       <c r="U12" s="60"/>
       <c r="V12" s="61"/>
@@ -1764,26 +1813,26 @@
       <c r="AB12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="51" t="n">
+      <c r="B13" s="52" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="58"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="58"/>
+      <c r="C13" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="59"/>
       <c r="T13" s="10"/>
       <c r="U13" s="60"/>
       <c r="V13" s="61"/>
@@ -1795,26 +1844,26 @@
       <c r="AB13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="51" t="n">
+      <c r="B14" s="52" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="58"/>
+      <c r="C14" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="59"/>
       <c r="T14" s="10"/>
       <c r="U14" s="60"/>
       <c r="V14" s="61"/>
@@ -1826,81 +1875,82 @@
       <c r="AB14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="51"/>
+      <c r="B15" s="52"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="51"/>
+      <c r="B16" s="52"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="51"/>
+      <c r="B17" s="52"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="51"/>
+      <c r="B18" s="52"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="51"/>
+      <c r="B19" s="52"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="51"/>
+      <c r="B20" s="52"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="51"/>
+      <c r="B21" s="52"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="51"/>
+      <c r="B22" s="52"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="51"/>
+      <c r="B23" s="52"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="51"/>
+      <c r="B24" s="52"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="51"/>
+      <c r="B25" s="52"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="51"/>
+      <c r="B26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="51"/>
+      <c r="B27" s="52"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="51"/>
+      <c r="B28" s="52"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="51"/>
+      <c r="B29" s="52"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="51"/>
+      <c r="B30" s="52"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="51"/>
+      <c r="B31" s="52"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="51"/>
+      <c r="B32" s="52"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="51"/>
+      <c r="B33" s="52"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="51"/>
+      <c r="B34" s="52"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="51"/>
+      <c r="B35" s="52"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="51"/>
+      <c r="B36" s="52"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="51"/>
+      <c r="B37" s="52"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="51"/>
+      <c r="B38" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:AA1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
@@ -1912,59 +1962,67 @@
     <mergeCell ref="V4:AA4"/>
     <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA14" type="list">
+  <dataValidations count="14">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6:H14" type="list">
       <formula1>"Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C14 G6:G14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:T14" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T6 AB6:AD6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:S14" type="decimal">
+      <formula1>10</formula1>
+      <formula2>400</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B38" type="whole">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R14" type="list">
       <formula1>"Manual,Automatic"</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="decimal">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U14" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:U14" type="decimal">
       <formula1>10</formula1>
-      <formula2>400</formula2>
+      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1972,4 +2030,80 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:C2 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="65" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>